<commit_message>
Included Procfile for heroku
</commit_message>
<xml_diff>
--- a/log/logbook.xlsx
+++ b/log/logbook.xlsx
@@ -361,13 +361,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="17"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="14.6640625"/>
@@ -1061,6 +1061,66 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>43809.22349537037</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>jetnew</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>No content found.</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>43809.22594907408</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>jetnew</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>No content found.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
+        <v>43809.22703703704</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>jetnew</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>how long do students live in cinnamon college?</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>two years</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Reduced size of bert model to reduce memory
</commit_message>
<xml_diff>
--- a/log/logbook.xlsx
+++ b/log/logbook.xlsx
@@ -361,7 +361,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -1121,6 +1121,146 @@
         </is>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>43809.25942129629</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>jetnew</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>No content found.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
+        <v>43809.26697916666</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>jetnew</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>how long do students live in cinnamon college?</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>No content found.</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="n">
+        <v>43809.26760416666</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>jetnew</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>No content found.</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>43809.26768518519</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>jetnew</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>how long do students live in cinnamon college?</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>No content found.</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>43809.27247685185</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>jetnew</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>how long do students live in cinnamon college?</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>No content found.</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
+        <v>43809.27306712963</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>jetnew</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>how much credits do usp students earn in their home faculty?</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>$4000</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>43809.27318287037</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>jetnew</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>What does it mean to be curious?</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>No content found.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
try with a smaller model
</commit_message>
<xml_diff>
--- a/log/logbook.xlsx
+++ b/log/logbook.xlsx
@@ -361,7 +361,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -1261,6 +1261,66 @@
         </is>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>43810.45908564814</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>jetnew</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>No content found.</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>43810.45924768518</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>jetnew</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>What does it mean to be curious?</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>No content found.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="n">
+        <v>43810.45946759259</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>jetnew</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>how long do students live in cinnamon college?</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>No content found.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>